<commit_message>
First final implementation of Stationary Simulation
</commit_message>
<xml_diff>
--- a/config/default_DCDC.xlsx
+++ b/config/default_DCDC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f215465b21b5e6e2/Studium/34_Github/PyPowerSim/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="333" documentId="13_ncr:1_{28BD4CF4-A877-4909-81F4-E5A6CEB4DAD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CCB6F9E9-BC6E-4AB1-9272-BA8BE98F2B64}"/>
+  <xr:revisionPtr revIDLastSave="345" documentId="13_ncr:1_{28BD4CF4-A877-4909-81F4-E5A6CEB4DAD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48CBC987-73BA-4016-973F-69B0F9A74C96}"/>
   <bookViews>
-    <workbookView xWindow="-18120" yWindow="-2550" windowWidth="18240" windowHeight="28320" activeTab="4" xr2:uid="{DB7D2548-4471-4992-93B1-3EC0BA66F7EA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{DB7D2548-4471-4992-93B1-3EC0BA66F7EA}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="2" r:id="rId1"/>
@@ -748,9 +748,6 @@
   </si>
   <si>
     <t>0127</t>
-  </si>
-  <si>
-    <t>none</t>
   </si>
   <si>
     <t>23.06.2024</t>
@@ -919,6 +916,9 @@
   </si>
   <si>
     <t>TraMdl</t>
+  </si>
+  <si>
+    <t>none</t>
   </si>
 </sst>
 </file>
@@ -1555,10 +1555,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1879,7 +1875,7 @@
         <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -1895,7 +1891,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -1903,7 +1899,7 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1927,7 +1923,7 @@
         <v>15</v>
       </c>
       <c r="J13" s="67" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K13" s="68"/>
       <c r="L13" s="69"/>
@@ -1952,13 +1948,13 @@
         <v>16</v>
       </c>
       <c r="J14" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="K14" s="39" t="s">
         <v>231</v>
       </c>
-      <c r="K14" s="39" t="s">
+      <c r="L14" s="40" t="s">
         <v>232</v>
-      </c>
-      <c r="L14" s="40" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -1982,10 +1978,10 @@
       </c>
       <c r="J15" s="41"/>
       <c r="K15" t="s">
+        <v>233</v>
+      </c>
+      <c r="L15" s="42" t="s">
         <v>234</v>
-      </c>
-      <c r="L15" s="42" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -1993,13 +1989,13 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C16" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E16" t="s">
         <v>16</v>
@@ -2009,10 +2005,10 @@
       </c>
       <c r="J16" s="43"/>
       <c r="K16" t="s">
+        <v>236</v>
+      </c>
+      <c r="L16" s="42" t="s">
         <v>237</v>
-      </c>
-      <c r="L16" s="42" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -2020,13 +2016,13 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
+        <v>254</v>
+      </c>
+      <c r="C17" t="s">
         <v>255</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>256</v>
-      </c>
-      <c r="D17" t="s">
-        <v>257</v>
       </c>
       <c r="E17" t="s">
         <v>16</v>
@@ -2036,10 +2032,10 @@
       </c>
       <c r="J17" s="44"/>
       <c r="K17" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L17" s="42" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2048,10 +2044,10 @@
       </c>
       <c r="J18" s="45"/>
       <c r="K18" s="46" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L18" s="47" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -2067,8 +2063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CAB857B-5D2E-4BE1-B462-B4B5EEAA4370}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2147,7 +2143,7 @@
         <v>37</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>227</v>
+        <v>266</v>
       </c>
       <c r="F4" s="55" t="s">
         <v>22</v>
@@ -2263,7 +2259,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2454,16 +2450,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B10" s="48" t="s">
         <v>56</v>
       </c>
       <c r="C10" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="D10" s="51" t="s">
         <v>259</v>
-      </c>
-      <c r="D10" s="51" t="s">
-        <v>260</v>
       </c>
       <c r="E10" s="11">
         <v>30</v>
@@ -2659,7 +2655,7 @@
         <v>96</v>
       </c>
       <c r="E2" s="36" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F2" s="57" t="s">
         <v>22</v>
@@ -2667,7 +2663,7 @@
     </row>
     <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="61" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B3" s="50"/>
       <c r="C3" s="17" t="s">
@@ -2685,7 +2681,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="62" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B4" s="48"/>
       <c r="C4" s="9" t="s">
@@ -2703,7 +2699,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="62" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B5" s="48"/>
       <c r="C5" s="9" t="s">
@@ -2721,7 +2717,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="62" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B6" s="48"/>
       <c r="C6" s="9" t="s">
@@ -2739,7 +2735,7 @@
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="62" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B7" s="48"/>
       <c r="C7" s="10" t="s">
@@ -2757,7 +2753,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="62" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B8" s="48"/>
       <c r="C8" s="9" t="s">
@@ -2775,7 +2771,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="62" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B9" s="48"/>
       <c r="C9" s="9" t="s">
@@ -2793,7 +2789,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="62" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B10" s="48"/>
       <c r="C10" s="9" t="s">
@@ -2811,7 +2807,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="62" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B11" s="48"/>
       <c r="C11" s="9" t="s">
@@ -2829,11 +2825,11 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="62" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B12" s="48"/>
       <c r="C12" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D12" s="51" t="s">
         <v>107</v>
@@ -2847,7 +2843,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="62" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B13" s="48"/>
       <c r="C13" s="9" t="s">
@@ -2865,7 +2861,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="62" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B14" s="48"/>
       <c r="C14" s="9" t="s">
@@ -2883,11 +2879,11 @@
     </row>
     <row r="15" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="62" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B15" s="48"/>
       <c r="C15" s="10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D15" s="51" t="s">
         <v>110</v>
@@ -2901,7 +2897,7 @@
     </row>
     <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="63" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B16" s="49"/>
       <c r="C16" s="14" t="s">
@@ -2946,7 +2942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245B3F0A-B85A-4162-A12D-AC7176B54015}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
@@ -2985,13 +2981,13 @@
         <v>138</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D2" s="53" t="s">
         <v>34</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F2" s="56" t="s">
         <v>22</v>
@@ -3249,7 +3245,7 @@
         <v>34</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F15" s="56" t="s">
         <v>22</v>
@@ -3497,7 +3493,7 @@
     </row>
     <row r="28" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="33" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B28" s="65" t="s">
         <v>162</v>
@@ -3506,7 +3502,7 @@
         <v>187</v>
       </c>
       <c r="D28" s="51" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E28" s="18" t="s">
         <v>167</v>

</xml_diff>